<commit_message>
add quiz and notes
</commit_message>
<xml_diff>
--- a/Course 3 Prepare data for exploration/Import HTML.xlsx
+++ b/Course 3 Prepare data for exploration/Import HTML.xlsx
@@ -1,13 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\google analytic-20220922T235135Z-001\google analytic\Course 3 Prepare data for exploration\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14855FB5-D7C5-4EAD-8E0D-B65C9143FC6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -20,26 +40,30 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF1F1F1F"/>
       <name val="&quot;Source Sans Pro&quot;"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -47,7 +71,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -57,41 +81,44 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="3" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="10" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -281,22 +308,25 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTHTML(""http://en.wikipedia.org/wiki/Demographics_of_India"",""table"",1)"),"Demographics of India")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IMPORTHTML(""http://en.wikipedia.org/wiki/Demographics_of_India"",""table"",1)"),"Demographics of India")</f>
         <v>Demographics of India</v>
       </c>
       <c r="B1" s="2"/>
@@ -304,248 +334,248 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"India population pyramid in 2020")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"India population pyramid in 2020")</f>
         <v>India population pyramid in 2020</v>
       </c>
       <c r="B2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Population")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Population")</f>
         <v>Population</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1,407,563,842[1] (2021 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1,407,563,842[1] (2021 est.)")</f>
         <v>1,407,563,842[1] (2021 est.)</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Density")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Density")</f>
         <v>Density</v>
       </c>
       <c r="B4" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"473.42 people per.km2 (2021 est.)[2]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"473.42 people per.km2 (2021 est.)[2]")</f>
         <v>473.42 people per.km2 (2021 est.)[2]</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:6">
       <c r="A5" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Growth rate")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Growth rate")</f>
         <v>Growth rate</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0.68% (2021 est.)[3]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0.68% (2021 est.)[3]")</f>
         <v>0.68% (2021 est.)[3]</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:6">
       <c r="A6" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Birth rate")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Birth rate")</f>
         <v>Birth rate</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"16.42 births/1,000 population (2021 est.)[4]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"16.42 births/1,000 population (2021 est.)[4]")</f>
         <v>16.42 births/1,000 population (2021 est.)[4]</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:6">
       <c r="A7" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Death rate")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Death rate")</f>
         <v>Death rate</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"9.45 deaths/1,000 population (2021 est.)[5]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"9.45 deaths/1,000 population (2021 est.)[5]")</f>
         <v>9.45 deaths/1,000 population (2021 est.)[5]</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:6">
       <c r="A8" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Life expectancy")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Life expectancy")</f>
         <v>Life expectancy</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"67.2 years (2021 est.)[6]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"67.2 years (2021 est.)[6]")</f>
         <v>67.2 years (2021 est.)[6]</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:6">
       <c r="A9" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"• male")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"• male")</f>
         <v>• male</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65.8 years (2021 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65.8 years (2021 est.)")</f>
         <v>65.8 years (2021 est.)</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:6">
       <c r="A10" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"• female")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"• female")</f>
         <v>• female</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"68.9 years (2020 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"68.9 years (2020 est.)")</f>
         <v>68.9 years (2020 est.)</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:6">
       <c r="A11" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Fertility rate")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Fertility rate")</f>
         <v>Fertility rate</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"2.03 children born per woman (2021)[7]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"2.03 children born per woman (2021)[7]")</f>
         <v>2.03 children born per woman (2021)[7]</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Infant mortality rate")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Infant mortality rate")</f>
         <v>Infant mortality rate</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"29.94 deaths/1,000 live births (2018)[8]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"29.94 deaths/1,000 live births (2018)[8]")</f>
         <v>29.94 deaths/1,000 live births (2018)[8]</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:6">
       <c r="A13" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Age structure")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Age structure")</f>
         <v>Age structure</v>
       </c>
       <c r="B13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0–14 years")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0–14 years")</f>
         <v>0–14 years</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"28.6% (male 190,075,427/female 172,799,553)[9]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"28.6% (male 190,075,427/female 172,799,553)[9]")</f>
         <v>28.6% (male 190,075,427/female 172,799,553)[9]</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"15–64 years")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"15–64 years")</f>
         <v>15–64 years</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"63.6% (male 381,446,079/female 359,802,209) (2009 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"63.6% (male 381,446,079/female 359,802,209) (2009 est.)")</f>
         <v>63.6% (male 381,446,079/female 359,802,209) (2009 est.)</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65 and over")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65 and over")</f>
         <v>65 and over</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"5.3% (male 29,364,920/female 32,591,030) (2009 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"5.3% (male 29,364,920/female 32,591,030) (2009 est.)")</f>
         <v>5.3% (male 29,364,920/female 32,591,030) (2009 est.)</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:2">
       <c r="A17" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sex ratio")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Sex ratio")</f>
         <v>Sex ratio</v>
       </c>
       <c r="B17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:2">
       <c r="A18" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Total")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Total")</f>
         <v>Total</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.079 male(s)/female (2020)[10]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.079 male(s)/female (2020)[10]")</f>
         <v>1.079 male(s)/female (2020)[10]</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:2">
       <c r="A19" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"At birth")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"At birth")</f>
         <v>At birth</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.11 male(s)/female (2020)[10]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.11 male(s)/female (2020)[10]")</f>
         <v>1.11 male(s)/female (2020)[10]</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:2">
       <c r="A20" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Under 15")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Under 15")</f>
         <v>Under 15</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0–14 years: 1.13 male(s)/female (2020)[10]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0–14 years: 1.13 male(s)/female (2020)[10]")</f>
         <v>0–14 years: 1.13 male(s)/female (2020)[10]</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:2">
       <c r="A21" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"15–64 years")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"15–64 years")</f>
         <v>15–64 years</v>
       </c>
       <c r="B21" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.06 male(s)/female (2009 est.)")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1.06 male(s)/female (2009 est.)")</f>
         <v>1.06 male(s)/female (2009 est.)</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:2">
       <c r="A22" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65 and over")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"65 and over")</f>
         <v>65 and over</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0.89 male(s)/female (2020)[10]")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"0.89 male(s)/female (2020)[10]")</f>
         <v>0.89 male(s)/female (2020)[10]</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:2">
       <c r="A23" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Nationality")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Nationality")</f>
         <v>Nationality</v>
       </c>
       <c r="B23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:2">
       <c r="A24" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Major ethnic")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Major ethnic")</f>
         <v>Major ethnic</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"See Ethnic groups of India")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"See Ethnic groups of India")</f>
         <v>See Ethnic groups of India</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:2">
       <c r="A25" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Language")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Language")</f>
         <v>Language</v>
       </c>
       <c r="B25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:2">
       <c r="A26" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Official")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Official")</f>
         <v>Official</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"See Languages of India")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"See Languages of India")</f>
         <v>See Languages of India</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:2">
       <c r="A27" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Spoken")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Spoken")</f>
         <v>Spoken</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"- Hindi 43.6%[note 1]
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"- Hindi 43.6%[note 1]
    - Bengali 8%
    - Marathi 6.9%
    - Telugu 6.8%
@@ -579,38 +609,39 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F1"/>
+    <hyperlink ref="F1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("IMPORTHTML(""http://en.wikipedia.org/wiki/Demographics_of_India"",""table"",2)"),"Year")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("IMPORTHTML(""http://en.wikipedia.org/wiki/Demographics_of_India"",""table"",2)"),"Year")</f>
         <v>Year</v>
       </c>
       <c r="B1" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Aggregate average")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Aggregate average")</f>
         <v>Aggregate average</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Period")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Period")</f>
         <v>Period</v>
       </c>
       <c r="E1" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Average 
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Average 
  % growth 
 / century")</f>
         <v>Average 
@@ -618,217 +649,217 @@
 / century</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" s="2"/>
       <c r="B2" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Population")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Population")</f>
         <v>Population</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"% of World population")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"% of World population")</f>
         <v>% of World population</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"10,000 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"10,000 BC")</f>
         <v>10,000 BC</v>
       </c>
       <c r="B3" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000)</f>
         <v>1000</v>
       </c>
       <c r="C3" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0083)</f>
-        <v>0.0083</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.0083)</f>
+        <v>8.3000000000000001E-3</v>
       </c>
       <c r="D3" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Stone Age")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Stone Age")</f>
         <v>Stone Age</v>
       </c>
       <c r="E3" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),30.28)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),30.28)</f>
         <v>30.28</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"4000 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"4000 BC")</f>
         <v>4000 BC</v>
       </c>
       <c r="B4" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000000.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000000)</f>
         <v>1000000</v>
       </c>
       <c r="C4" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3083)</f>
-        <v>0.3083</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3083)</f>
+        <v>0.30830000000000002</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"2000 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"2000 BC")</f>
         <v>2000 BC</v>
       </c>
       <c r="B5" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.3E7)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),13000000)</f>
         <v>13000000</v>
       </c>
       <c r="C5" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.37143)</f>
-        <v>0.37143</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.37143)</f>
+        <v>0.37142999999999998</v>
       </c>
       <c r="D5" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Bronze Age")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Bronze Age")</f>
         <v>Bronze Age</v>
       </c>
       <c r="E5" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.25)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),26.25)</f>
         <v>26.25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"500 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"500 BC")</f>
         <v>500 BC</v>
       </c>
       <c r="B6" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),8.34E7)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),83400000)</f>
         <v>83400000</v>
       </c>
       <c r="C6" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.417)</f>
-        <v>0.417</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.417)</f>
+        <v>0.41699999999999998</v>
       </c>
       <c r="D6" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Iron Age")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Iron Age")</f>
         <v>Iron Age</v>
       </c>
       <c r="E6" s="2"/>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"400 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"400 BC")</f>
         <v>400 BC</v>
       </c>
       <c r="B7" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.026E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),102600000)</f>
         <v>102600000</v>
       </c>
       <c r="C7" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4396)</f>
-        <v>0.4396</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4396)</f>
+        <v>0.43959999999999999</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"200 BC")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"200 BC")</f>
         <v>200 BC</v>
       </c>
       <c r="B8" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.429E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),142900000)</f>
         <v>142900000</v>
       </c>
       <c r="C8" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4763)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4763)</f>
         <v>0.4763</v>
       </c>
       <c r="D8" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Maurya era")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Maurya era")</f>
         <v>Maurya era</v>
       </c>
       <c r="E8" s="2"/>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1 AD")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"1 AD")</f>
         <v>1 AD</v>
       </c>
       <c r="B9" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.667E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),166700000)</f>
         <v>166700000</v>
       </c>
       <c r="C9" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3556)</f>
-        <v>0.3556</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3556)</f>
+        <v>0.35560000000000003</v>
       </c>
       <c r="D9" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Classical 
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Classical 
 era")</f>
         <v>Classical 
 era</v>
       </c>
       <c r="E9" s="2"/>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),200.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),200)</f>
         <v>200</v>
       </c>
       <c r="B10" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),200000000)</f>
         <v>200000000</v>
       </c>
       <c r="C10" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3615)</f>
-        <v>0.3615</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3615)</f>
+        <v>0.36149999999999999</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),400.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),400)</f>
         <v>400</v>
       </c>
       <c r="B11" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.5E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),250000000)</f>
         <v>250000000</v>
       </c>
       <c r="C11" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4)</f>
         <v>0.4</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),500.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),500)</f>
         <v>500</v>
       </c>
       <c r="B12" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.858E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),285800000)</f>
         <v>285800000</v>
       </c>
       <c r="C12" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4358)</f>
-        <v>0.4358</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4358)</f>
+        <v>0.43580000000000002</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),600.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),600)</f>
         <v>600</v>
       </c>
       <c r="B13" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.334E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),333400000)</f>
         <v>333400000</v>
       </c>
       <c r="C13" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4883)</f>
-        <v>0.4883</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.4883)</f>
+        <v>0.48830000000000001</v>
       </c>
       <c r="D13" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Early 
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Early 
 medieval 
 era")</f>
         <v>Early 
@@ -837,85 +868,85 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),700.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),700)</f>
         <v>700</v>
       </c>
       <c r="B14" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),4.0E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),400000000)</f>
         <v>400000000</v>
       </c>
       <c r="C14" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5667)</f>
-        <v>0.5667</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5667)</f>
+        <v>0.56669999999999998</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),800.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),800)</f>
         <v>800</v>
       </c>
       <c r="B15" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.9E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),390000000)</f>
         <v>390000000</v>
       </c>
       <c r="C15" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.55)</f>
-        <v>0.55</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.55)</f>
+        <v>0.55000000000000004</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),900.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),900)</f>
         <v>900</v>
       </c>
       <c r="B16" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.8E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),380000000)</f>
         <v>380000000</v>
       </c>
       <c r="C16" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5334)</f>
-        <v>0.5334</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.5334)</f>
+        <v>0.53339999999999999</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1000)</f>
         <v>1000</v>
       </c>
       <c r="B17" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.6E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),360000000)</f>
         <v>360000000</v>
       </c>
       <c r="C17" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3)</f>
         <v>0.3</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1100.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1100)</f>
         <v>1100</v>
       </c>
       <c r="B18" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),3.3E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),330000000)</f>
         <v>330000000</v>
       </c>
       <c r="C18" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.35)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.35)</f>
         <v>0.35</v>
       </c>
       <c r="D18" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Late 
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Late 
 medieval 
 era")</f>
         <v>Late 
@@ -924,170 +955,170 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1200.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1200)</f>
         <v>1200</v>
       </c>
       <c r="B19" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.8E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),280000000)</f>
         <v>280000000</v>
       </c>
       <c r="C19" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3667)</f>
-        <v>0.3667</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3667)</f>
+        <v>0.36670000000000003</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1300.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1300)</f>
         <v>1300</v>
       </c>
       <c r="B20" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.3E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),230000000)</f>
         <v>230000000</v>
       </c>
       <c r="C20" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3834)</f>
-        <v>0.3834</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3834)</f>
+        <v>0.38340000000000002</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1400.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1400)</f>
         <v>1400</v>
       </c>
       <c r="B21" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.8E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),180000000)</f>
         <v>180000000</v>
       </c>
       <c r="C21" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.3)</f>
         <v>0.3</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1500.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1500)</f>
         <v>1500</v>
       </c>
       <c r="B22" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.3E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),130000000)</f>
         <v>130000000</v>
       </c>
       <c r="C22" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2167)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2167)</f>
         <v>0.2167</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5">
       <c r="A23" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1600.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1600)</f>
         <v>1600</v>
       </c>
       <c r="B23" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.4E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),140000000)</f>
         <v>140000000</v>
       </c>
       <c r="C23" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2333)</f>
-        <v>0.2333</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2333)</f>
+        <v>0.23330000000000001</v>
       </c>
       <c r="D23" s="2" t="str">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Early modern era")</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),"Early modern era")</f>
         <v>Early modern era</v>
       </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1650.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1650)</f>
         <v>1650</v>
       </c>
       <c r="B24" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.7E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),170000000)</f>
         <v>170000000</v>
       </c>
       <c r="C24" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2615)</f>
-        <v>0.2615</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2615)</f>
+        <v>0.26150000000000001</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1700.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1700)</f>
         <v>1700</v>
       </c>
       <c r="B25" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.4E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),140000000)</f>
         <v>140000000</v>
       </c>
       <c r="C25" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2)</f>
         <v>0.2</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26">
+    <row r="26" spans="1:5">
       <c r="A26" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1750.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1750)</f>
         <v>1750</v>
       </c>
       <c r="B26" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1.83E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),183000000)</f>
         <v>183000000</v>
       </c>
       <c r="C26" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2153)</f>
-        <v>0.2153</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2153)</f>
+        <v>0.21529999999999999</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27">
+    <row r="27" spans="1:5">
       <c r="A27" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1800.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1800)</f>
         <v>1800</v>
       </c>
       <c r="B27" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.0E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),200000000)</f>
         <v>200000000</v>
       </c>
       <c r="C27" s="6">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.2)</f>
         <v>0.2</v>
       </c>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28">
+    <row r="28" spans="1:5">
       <c r="A28" s="2">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1820.0)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),1820)</f>
         <v>1820</v>
       </c>
       <c r="B28" s="4">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),2.1E8)</f>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),210000000)</f>
         <v>210000000</v>
       </c>
       <c r="C28" s="5">
-        <f>IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.1909)</f>
-        <v>0.1909</v>
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("""COMPUTED_VALUE"""),0.1909)</f>
+        <v>0.19089999999999999</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>